<commit_message>
Ashley updates and date.
</commit_message>
<xml_diff>
--- a/_site/Data/FamConf.xlsx
+++ b/_site/Data/FamConf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abautist/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA1C757-B12A-264F-9E21-B6FD6C9AFF77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F396AC-1BF6-BD4A-B090-0C4D44C48F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6220" yWindow="460" windowWidth="24740" windowHeight="15540" xr2:uid="{8A673D2B-23AC-4849-B85E-D6BED00A64B1}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="19160" windowHeight="21140" xr2:uid="{8A673D2B-23AC-4849-B85E-D6BED00A64B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Question Bank " sheetId="1" r:id="rId1"/>
@@ -25,16 +25,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Question</t>
   </si>
   <si>
-    <t>Past</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Families have many different ways of trying to settle their differences. This is a list of things that might happen when your family has differences. Please mark how many times each of these things happened in the last week. Please also think about a typical week in your family’s like prior to the coronavirus (COVID-19) pandemic, and mark how many times each of these things happened. If one of these things did not occur, then select “This has not happened" for that question. If a question does not apply to your family, then select “NA”.   
-In the last week… &amp; In a typical week prior to the COVID-19 Pandemic... (Answer Choices: Once per week, Twice per week, 3-5 times per week, 6-10 times per week, More than 10 times per week, This has not happened, N/A) 
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Occurrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Once per week
+• Twice per week
+• 3-5 times per week
+• 6-10 times per week
+• More than 10 times per week
+• This has not happened
+• Not applicable </t>
+  </si>
+  <si>
+    <t>• being confident that my family has health insurance 
+• not being so socially isolated 
+• having lower levels of worry and stress 
+• knowing we can pay for food  
+• knowing we can pay my rent/mortgage/housing expenses 
+• knowing my/our job is secure 
+• being able to meet my child’s social and emotional needs 
+• knowing we have access to childcare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Think about the sources of conflict for your family. Which of the following would help decrease conflict the most right now? </t>
+  </si>
+  <si>
+    <t>• Once per week
+• Twice per week
+• 3-5 times per week
+• 6-10 times per week
+• More than 10 times per week
+• This has not happened
+• N/A</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Families have many different ways of trying to settle their differences. This is a list of things that might happen when your family has differences. Please mark how many times each of these things happened in the last week. Please also think about a typical week in your family’s life prior to the coronavirus (COVID-19) pandemic, and mark how many times each of these things happened. If one of these things did not occur, then select “This has not happened" for that question. If a question does not apply to your family, then select “NA”.   
+In a typical week </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prior to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the COVID-19 Pandemic.
 • I insulted or swore or shouted or yelled at my partner  
 • I shouted, yelled, or screamed at my child  
 • I criticized or said mean things to my child 
@@ -45,36 +101,134 @@
 • My child had a temper tantrum  
 • My child argued with me  
 • My child argued with my partner </t>
-  </si>
-  <si>
-    <t>When you and your child have spent time together, how often did you do the following? If one of these things did not occur, then select “This has not happened" for that question. If a question does not apply to your family, then select “NA”. 
-In the last week… &amp; In a typical week prior to the COVID-19 Pandemic... (Answer Choices: Once per week, Twice per week, 3-5 times per week, 6-10 times per week, More than 10 times per week, This has not happened, N/A) 
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>When you and your child have spent time together, how often did you do the following? If one of these things did not occur, then select “This has not happened" for that question. If a question does not apply to your family, then select “NA”. 
+In a typical week</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> prior to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">the COVID-19 Pandemic...
 • I let my child know I really care about them 
 • I was loving and affectionate toward my child 
 • I was supportive and understanding toward my child 
 • I told my child I love them 
-Think about the sources of conflict for your family. Which of the following would help decrease conflict the most right now? 
-• being confident that my family has health insurance 
-• not being so socially isolated 
-• having lower levels of worry and stress 
-• knowing we can pay for food  
-• knowing we can pay my rent/mortgage/housing expenses 
-• knowing my/our job is secure 
-• being able to meet my child’s social and emotional needs 
-• knowing we have access to childcare</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Occurrence</t>
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed by RAPID-EC Team </t>
+  </si>
+  <si>
+    <t>Developed by RAPID Team
+- Interpersonal Conflict: Conflict Tactics Scale, Revised, Short form CTS25
+- Harsh Parenting: Conflict Tactics Scale Parent-Child and Iowa Family Interaction Rating Scales (WH)
+- Child Behavior: Early Childhood Behavior Questionnaire</t>
+  </si>
+  <si>
+    <t>RAPID Team Modified
+Iowa Family Interaction Rating Scales (WH)</t>
+  </si>
+  <si>
+    <t>Past
+9, 11, 16</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Families have many different ways of trying to settle their differences. This is a list of things that might happen when your family has differences. Please mark how many times each of these things happened in the last week. Please also think about a typical week in your family’s life prior to the coronavirus (COVID-19) pandemic, and mark how many times each of these things happened. If one of these things did not occur, then select “This has not happened" for that question. If a question does not apply to your family, then select “NA”.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+In the last week…</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• I insulted or swore or shouted or yelled at my partner  
+• I shouted, yelled, or screamed at my child  
+• I criticized or said mean things to my child 
+• I felt like throwing things or slamming doors 
+• My partner insulted or swore or shouted or yelled at me 
+• My partner shouted, yelled, or screamed at my child 
+• My partner criticized my child  
+• My child had a temper tantrum  
+• My child argued with me  
+• My child argued with my partner </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When you and your child have spent time together, how often did you do the following? If one of these things did not occur, then select “This has not happened" for that question. If a question does not apply to your family, then select “NA”. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+In the last week…</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• I let my child know I really care about them 
+• I was loving and affectionate toward my child 
+• I was supportive and understanding toward my child 
+• I told my child I love them </t>
+    </r>
+  </si>
+  <si>
+    <t>Answers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,6 +237,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -110,11 +280,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,46 +615,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2689D1A7-E07D-A54D-BF8D-68ACF4A3D5C5}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="75" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="1" max="2" width="75" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="323" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="323" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="356">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="372">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>